<commit_message>
physics simulation analysis, go fish analysis
</commit_message>
<xml_diff>
--- a/rps_data/entropy_dummy.xlsx
+++ b/rps_data/entropy_dummy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikbrockbank/web/vullab/data_analysis/rps_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC76F74E-73DC-A047-987C-19A28DE7E634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CF7B15-F2B5-8B45-AB1C-2AAFD7F319EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{744D657E-4EE1-F249-8206-87D279D403C1}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -664,15 +664,15 @@
         <v>13</v>
       </c>
       <c r="I3" s="1">
-        <f>F3/SUM($F3:$H3)</f>
+        <f t="shared" ref="I3:K4" si="0">F3/SUM($F3:$H3)</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="J3" s="1">
-        <f>G3/SUM($F3:$H3)</f>
+        <f t="shared" si="0"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="K3" s="1">
-        <f>H3/SUM($F3:$H3)</f>
+        <f t="shared" si="0"/>
         <v>0.3611111111111111</v>
       </c>
       <c r="L3" s="7">
@@ -713,34 +713,34 @@
         <v>8</v>
       </c>
       <c r="I4" s="1">
-        <f>F4/SUM($F4:$H4)</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="J4" s="1">
-        <f>G4/SUM($F4:$H4)</f>
+        <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
       <c r="K4" s="1">
-        <f>H4/SUM($F4:$H4)</f>
+        <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
       <c r="L4" s="7">
         <v>25</v>
       </c>
       <c r="M4" s="15">
-        <f t="shared" ref="M4:M6" si="0">SUM(F4:H4)</f>
+        <f t="shared" ref="M4:M6" si="1">SUM(F4:H4)</f>
         <v>25</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" ref="N4:N11" si="1">L4/$B$13</f>
+        <f t="shared" ref="N4:N11" si="2">L4/$B$13</f>
         <v>8.3612040133779264E-2</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" ref="O4:O11" si="2">-SUM(I4*LOG(I4, 2),J4*LOG(J4, 2), K4*LOG(K4, 2))</f>
+        <f t="shared" ref="O4:O11" si="3">-SUM(I4*LOG(I4, 2),J4*LOG(J4, 2), K4*LOG(K4, 2))</f>
         <v>1.4986885704510973</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P11" si="3">O4*N4</f>
+        <f t="shared" ref="P4:P11" si="4">O4*N4</f>
         <v>0.12530840890059342</v>
       </c>
     </row>
@@ -770,26 +770,26 @@
         <v>0.48484848484848486</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" ref="K4:K11" si="4">H5/SUM($F5:$H5)</f>
+        <f t="shared" ref="K5:K11" si="5">H5/SUM($F5:$H5)</f>
         <v>0.48484848484848486</v>
       </c>
       <c r="L5" s="7">
         <v>33</v>
       </c>
       <c r="M5" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.11036789297658862</v>
       </c>
       <c r="O5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1656062405705747</v>
       </c>
       <c r="P5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.12864550481213699</v>
       </c>
     </row>
@@ -811,7 +811,7 @@
         <v>22</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" ref="I4:I11" si="5">F6/SUM($F6:$H6)</f>
+        <f t="shared" ref="I6:I11" si="6">F6/SUM($F6:$H6)</f>
         <v>0.37209302325581395</v>
       </c>
       <c r="J6" s="1">
@@ -819,26 +819,26 @@
         <v>0.11627906976744186</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.51162790697674421</v>
       </c>
       <c r="L6" s="7">
         <v>43</v>
       </c>
       <c r="M6" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.14381270903010032</v>
       </c>
       <c r="O6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3863313573891363</v>
       </c>
       <c r="P6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.19937206811950786</v>
       </c>
     </row>
@@ -860,15 +860,15 @@
         <v>8</v>
       </c>
       <c r="I7" s="1">
+        <f t="shared" si="6"/>
+        <v>0.52173913043478259</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" ref="J7:J11" si="7">G7/SUM($F7:$H7)</f>
+        <v>0.13043478260869565</v>
+      </c>
+      <c r="K7" s="1">
         <f t="shared" si="5"/>
-        <v>0.52173913043478259</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" ref="J4:J11" si="6">G7/SUM($F7:$H7)</f>
-        <v>0.13043478260869565</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" si="4"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="L7" s="7">
@@ -879,15 +879,15 @@
         <v>23</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="O7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4029342381953893</v>
       </c>
       <c r="P7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.10791801832272226</v>
       </c>
     </row>
@@ -909,34 +909,34 @@
         <v>22</v>
       </c>
       <c r="I8" s="1">
+        <f t="shared" si="6"/>
+        <v>0.43181818181818182</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="7"/>
+        <v>6.8181818181818177E-2</v>
+      </c>
+      <c r="K8" s="1">
         <f t="shared" si="5"/>
-        <v>0.43181818181818182</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="6"/>
-        <v>6.8181818181818177E-2</v>
-      </c>
-      <c r="K8" s="1">
-        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="L8" s="7">
         <v>44</v>
       </c>
       <c r="M8" s="15">
-        <f t="shared" ref="M8:M11" si="7">SUM(F8:H8)</f>
+        <f t="shared" ref="M8:M11" si="8">SUM(F8:H8)</f>
         <v>44</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.14715719063545152</v>
       </c>
       <c r="O8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2873178489188395</v>
       </c>
       <c r="P8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.18943807810176905</v>
       </c>
     </row>
@@ -958,34 +958,34 @@
         <v>2</v>
       </c>
       <c r="I9" s="1">
+        <f t="shared" si="6"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="1">
         <f t="shared" si="5"/>
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="J9" s="1">
-        <f t="shared" si="6"/>
-        <v>0.5</v>
-      </c>
-      <c r="K9" s="1">
-        <f t="shared" si="4"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L9" s="7">
         <v>48</v>
       </c>
       <c r="M9" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>48</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.16053511705685619</v>
       </c>
       <c r="O9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.206908425151817</v>
       </c>
       <c r="P9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.1937511853086529</v>
       </c>
     </row>
@@ -1007,34 +1007,34 @@
         <v>1</v>
       </c>
       <c r="I10" s="1">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="7"/>
+        <v>0.625</v>
+      </c>
+      <c r="K10" s="1">
         <f t="shared" si="5"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="J10" s="1">
-        <f t="shared" si="6"/>
-        <v>0.625</v>
-      </c>
-      <c r="K10" s="1">
-        <f t="shared" si="4"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L10" s="7">
         <v>24</v>
       </c>
       <c r="M10" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.0267558528428096E-2</v>
       </c>
       <c r="O10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1431558784658322</v>
       </c>
       <c r="P10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.1758331381872824E-2</v>
       </c>
     </row>
@@ -1056,34 +1056,34 @@
         <v>2</v>
       </c>
       <c r="I11" s="1">
+        <f t="shared" si="6"/>
+        <v>0.34782608695652173</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="7"/>
+        <v>0.56521739130434778</v>
+      </c>
+      <c r="K11" s="1">
         <f t="shared" si="5"/>
-        <v>0.34782608695652173</v>
-      </c>
-      <c r="J11" s="1">
-        <f t="shared" si="6"/>
-        <v>0.56521739130434778</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="4"/>
         <v>8.6956521739130432E-2</v>
       </c>
       <c r="L11" s="7">
         <v>23</v>
       </c>
       <c r="M11" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3015742892816131</v>
       </c>
       <c r="P11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.10012109917550871</v>
       </c>
     </row>
@@ -1108,9 +1108,7 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="7">
-        <v>0.51600000000000001</v>
-      </c>
+      <c r="B14" s="7"/>
     </row>
     <row r="17" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1133,17 +1131,17 @@
     <row r="19" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="13">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="C19" s="13">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="D19" s="13">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="E19" s="12">
         <f>-SUM(B19*LOG(B19, 2), C19*LOG(C19, 2), D19*LOG(D19, 2))</f>
-        <v>0.5689955935892812</v>
+        <v>1.5219280948873621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>